<commit_message>
Remove urlEndpoint, fix legal agreement, fix date in report (#9)
* Remove urlEndpoint, fix legal agreement, fix date in report

* Change sign extension

* CreatedAt to SignedAt

* Change date format to "dd.mm.yyyy"
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/provision_of_service_act.xlsx
+++ b/src/main/resources/templates/provision_of_service_act.xlsx
@@ -173,9 +173,6 @@
     <t>${fromTime}</t>
   </si>
   <si>
-    <t>${partyRepresentation.merchantContractCreatedAt}</t>
-  </si>
-  <si>
     <t>${partyRepresentation.merchantName}</t>
   </si>
   <si>
@@ -195,15 +192,17 @@
   </si>
   <si>
     <t>${shopAccounting.fundsRefunded}</t>
+  </si>
+  <si>
+    <t>${partyRepresentation.merchantContractSignedAt}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;;&quot;-&quot;#,##0.00&quot; &quot;"/>
-    <numFmt numFmtId="165" formatCode="[$-FC19]dd\ mmmm\ yyyy\ \г\.;@"/>
     <numFmt numFmtId="166" formatCode="dd\.mm\.yyyy"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
@@ -340,12 +339,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -358,6 +351,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -372,8 +368,11 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1565,7 +1564,7 @@
   <dimension ref="A1:DZ234"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1575,24 +1574,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:130" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="23"/>
+      <c r="A2" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
@@ -1602,13 +1601,13 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
     </row>
     <row r="5" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
@@ -1626,8 +1625,8 @@
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="22" t="s">
-        <v>41</v>
+      <c r="E6" s="20" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:130" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1769,7 +1768,7 @@
       <c r="C8" s="2"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1783,7 +1782,7 @@
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="13"/>
-      <c r="D10" s="21"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1822,13 +1821,13 @@
       <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="28" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="29" t="s">
         <v>38</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1857,7 +1856,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="18" t="s">
         <v>36</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -1868,7 +1867,7 @@
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="19"/>
+      <c r="D19" s="17"/>
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1877,7 +1876,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
       <c r="E20" s="5" t="s">
@@ -1908,12 +1907,12 @@
       <c r="E23"/>
     </row>
     <row r="24" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="20" t="s">
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="18" t="s">
         <v>34</v>
       </c>
       <c r="E24" s="5" t="s">
@@ -1921,12 +1920,12 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="20" t="s">
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="18" t="s">
         <v>36</v>
       </c>
       <c r="E25" s="5" t="s">
@@ -1934,12 +1933,12 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="20" t="s">
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="18" t="s">
         <v>37</v>
       </c>
       <c r="E26" s="5" t="s">
@@ -1947,25 +1946,25 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="20" t="s">
-        <v>46</v>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="20">
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="18">
         <v>0</v>
       </c>
       <c r="E28" s="5" t="s">
@@ -1973,25 +1972,25 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="20" t="s">
-        <v>47</v>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="18" t="s">
+        <v>46</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="20" t="s">
+      <c r="B30" s="23"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="18" t="s">
         <v>35</v>
       </c>
       <c r="E30" s="5" t="s">
@@ -2090,7 +2089,7 @@
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2119,7 +2118,7 @@
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Yet another fixes (#10)
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/provision_of_service_act.xlsx
+++ b/src/main/resources/templates/provision_of_service_act.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
   <si>
     <t>Акт об оказании услуг</t>
   </si>
@@ -183,9 +183,6 @@
   </si>
   <si>
     <t>${partyRepresentation.merchantRepresentativePosition} ${partyRepresentation.merchantRepresentativeFullName}</t>
-  </si>
-  <si>
-    <t>${partyRepresentation.merchantRepresentativeDocument}</t>
   </si>
   <si>
     <t>${shopAccounting.fundsPaidOut}</t>
@@ -203,7 +200,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;;&quot;-&quot;#,##0.00&quot; &quot;"/>
-    <numFmt numFmtId="166" formatCode="dd\.mm\.yyyy"/>
+    <numFmt numFmtId="165" formatCode="dd\.mm\.yyyy"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -352,8 +349,14 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -367,12 +370,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1564,7 +1561,7 @@
   <dimension ref="A1:DZ234"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1574,22 +1571,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:130" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="21"/>
     </row>
@@ -1601,13 +1598,13 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
@@ -1821,13 +1818,13 @@
       <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="23" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="24" t="s">
         <v>38</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1907,11 +1904,11 @@
       <c r="E23"/>
     </row>
     <row r="24" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
       <c r="D24" s="18" t="s">
         <v>34</v>
       </c>
@@ -1920,11 +1917,11 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="18" t="s">
         <v>36</v>
       </c>
@@ -1933,11 +1930,11 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="18" t="s">
         <v>37</v>
       </c>
@@ -1946,24 +1943,24 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="18">
         <v>0</v>
       </c>
@@ -1972,24 +1969,24 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
       <c r="D30" s="18" t="s">
         <v>35</v>
       </c>
@@ -2118,7 +2115,7 @@
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="10" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
REP-13: Move name in template (#17)
* REP-13: Move name in template

* REP-13: Bump version

* REP-13: Bump damsel, other fixes
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/provision_of_service_act.xlsx
+++ b/src/main/resources/templates/provision_of_service_act.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>Акт об оказании услуг</t>
   </si>
@@ -143,9 +143,6 @@
     <t>________________________</t>
   </si>
   <si>
-    <t>Председатель Правления Бурлаков К.В.</t>
-  </si>
-  <si>
     <t>действует на основании</t>
   </si>
   <si>
@@ -182,9 +179,6 @@
     <t>к Договору № ${partyRepresentation.merchantContractId} от</t>
   </si>
   <si>
-    <t>${partyRepresentation.merchantRepresentativePosition} ${partyRepresentation.merchantRepresentativeFullName}</t>
-  </si>
-  <si>
     <t>${shopAccounting.fundsPaidOut}</t>
   </si>
   <si>
@@ -192,6 +186,18 @@
   </si>
   <si>
     <t>${partyRepresentation.merchantContractSignedAt}</t>
+  </si>
+  <si>
+    <t>${partyRepresentation.merchantRepresentativePosition}</t>
+  </si>
+  <si>
+    <t>${partyRepresentation.merchantRepresentativeFullName}</t>
+  </si>
+  <si>
+    <t>Председатель Правления</t>
+  </si>
+  <si>
+    <t>Бурлаков К.В.</t>
   </si>
 </sst>
 </file>
@@ -1561,7 +1567,7 @@
   <dimension ref="A1:DZ234"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1581,12 +1587,12 @@
     </row>
     <row r="2" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
       <c r="D2" s="22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E2" s="21"/>
     </row>
@@ -1623,7 +1629,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="10"/>
       <c r="E6" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:130" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1765,7 +1771,7 @@
       <c r="C8" s="2"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1819,13 +1825,13 @@
         <v>8</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>10</v>
@@ -1854,7 +1860,7 @@
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>13</v>
@@ -1874,7 +1880,7 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>13</v>
@@ -1910,7 +1916,7 @@
       <c r="B24" s="25"/>
       <c r="C24" s="25"/>
       <c r="D24" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>13</v>
@@ -1923,7 +1929,7 @@
       <c r="B25" s="27"/>
       <c r="C25" s="27"/>
       <c r="D25" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>18</v>
@@ -1936,7 +1942,7 @@
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
       <c r="D26" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>18</v>
@@ -1949,7 +1955,7 @@
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
       <c r="D27" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>18</v>
@@ -1975,7 +1981,7 @@
       <c r="B29" s="27"/>
       <c r="C29" s="27"/>
       <c r="D29" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>13</v>
@@ -1988,7 +1994,7 @@
       <c r="B30" s="25"/>
       <c r="C30" s="25"/>
       <c r="D30" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>13</v>
@@ -2080,42 +2086,46 @@
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
+      <c r="A42" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
-      <c r="E42" s="8"/>
+      <c r="E42" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2127,13 +2137,13 @@
     </row>
     <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
New acts by contract id (#21)
* REP-27: Act registry

* Fix temolate name

* New acts by contract id

* Fix tests

* Added bold border

* Fixed after comments, added test

* Add retry count in test

* Added invoices request

* Added files

* Fixed test

* Added payment tool column

* Uncomment deleting file

* Merge configs, add timeout for mst

* Bump woody version

* Bump damsel
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/provision_of_service_act.xlsx
+++ b/src/main/resources/templates/provision_of_service_act.xlsx
@@ -152,61 +152,60 @@
     <t>м.п.</t>
   </si>
   <si>
-    <t>${shopAccounting.openingBalance}</t>
-  </si>
-  <si>
-    <t>${shopAccounting.closingBalance}</t>
-  </si>
-  <si>
-    <t>${shopAccounting.fundsAcquired}</t>
-  </si>
-  <si>
-    <t>${shopAccounting.feeCharged}</t>
-  </si>
-  <si>
-    <t>${toTime}</t>
-  </si>
-  <si>
-    <t>${fromTime}</t>
-  </si>
-  <si>
-    <t>${partyRepresentation.merchantName}</t>
-  </si>
-  <si>
-    <t>${partyRepresentation.merchantId}</t>
-  </si>
-  <si>
-    <t>к Договору № ${partyRepresentation.merchantContractId} от</t>
-  </si>
-  <si>
-    <t>${shopAccounting.fundsPaidOut}</t>
-  </si>
-  <si>
-    <t>${shopAccounting.fundsRefunded}</t>
-  </si>
-  <si>
-    <t>${partyRepresentation.merchantContractSignedAt}</t>
-  </si>
-  <si>
-    <t>${partyRepresentation.merchantRepresentativePosition}</t>
-  </si>
-  <si>
-    <t>${partyRepresentation.merchantRepresentativeFullName}</t>
-  </si>
-  <si>
     <t>Председатель Правления</t>
   </si>
   <si>
     <t>Бурлаков К.В.</t>
+  </si>
+  <si>
+    <t>${registered_name}</t>
+  </si>
+  <si>
+    <t>${party_id}</t>
+  </si>
+  <si>
+    <t>${from_time}</t>
+  </si>
+  <si>
+    <t>${to_time}</t>
+  </si>
+  <si>
+    <t>${funds_acquired}</t>
+  </si>
+  <si>
+    <t>${fee_charged}</t>
+  </si>
+  <si>
+    <t>${opening_balance}</t>
+  </si>
+  <si>
+    <t>${funds_paid_out}</t>
+  </si>
+  <si>
+    <t>${funds_refunded}</t>
+  </si>
+  <si>
+    <t>${closing_balance}</t>
+  </si>
+  <si>
+    <t>${representative_full_name}</t>
+  </si>
+  <si>
+    <t>${representative_position}</t>
+  </si>
+  <si>
+    <t>к Договору № ${legal_agreement_id} от</t>
+  </si>
+  <si>
+    <t>${legal_agreement_signed_at}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;;&quot;-&quot;#,##0.00&quot; &quot;"/>
-    <numFmt numFmtId="165" formatCode="dd\.mm\.yyyy"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -355,15 +354,6 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -376,6 +366,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1567,7 +1566,7 @@
   <dimension ref="A1:DZ234"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1577,22 +1576,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:130" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="22" t="s">
-        <v>44</v>
+      <c r="A2" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="27" t="s">
+        <v>48</v>
       </c>
       <c r="E2" s="21"/>
     </row>
@@ -1604,13 +1603,13 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
     </row>
     <row r="5" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
@@ -1629,7 +1628,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="10"/>
       <c r="E6" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:130" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1771,7 +1770,7 @@
       <c r="C8" s="2"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1824,14 +1823,14 @@
       <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="23" t="s">
-        <v>38</v>
+      <c r="B15" s="29" t="s">
+        <v>37</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="24" t="s">
-        <v>37</v>
+      <c r="D15" s="28" t="s">
+        <v>38</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>10</v>
@@ -1860,7 +1859,7 @@
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="18" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>13</v>
@@ -1880,7 +1879,7 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="18" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>13</v>
@@ -1910,50 +1909,50 @@
       <c r="E23"/>
     </row>
     <row r="24" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
       <c r="D24" s="18" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
       <c r="D25" s="18" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
       <c r="D26" s="18" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
       <c r="D27" s="18" t="s">
         <v>42</v>
       </c>
@@ -1962,11 +1961,11 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
       <c r="D28" s="18">
         <v>0</v>
       </c>
@@ -1975,11 +1974,11 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
       <c r="D29" s="18" t="s">
         <v>43</v>
       </c>
@@ -1988,13 +1987,13 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
       <c r="D30" s="18" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>13</v>
@@ -2086,24 +2085,24 @@
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add shop in report template, other fixes (#36)
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/provision_of_service_act.xlsx
+++ b/src/main/resources/templates/provision_of_service_act.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
   <si>
     <t>Акт об оказании услуг</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>${legal_agreement_signed_at}</t>
+  </si>
+  <si>
+    <t>Идентификатор магазина:</t>
+  </si>
+  <si>
+    <t>${shop_id}</t>
   </si>
 </sst>
 </file>
@@ -297,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -355,6 +361,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -367,14 +382,8 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1566,7 +1575,7 @@
   <dimension ref="A1:DZ234"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1576,21 +1585,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:130" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="27" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="22" t="s">
         <v>48</v>
       </c>
       <c r="E2" s="21"/>
@@ -1603,13 +1612,13 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
@@ -1777,15 +1786,19 @@
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
+      <c r="D9" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="30"/>
     </row>
     <row r="10" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="13"/>
       <c r="D10" s="19"/>
-      <c r="E10" s="13"/>
+      <c r="E10" s="13" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
@@ -1823,13 +1836,13 @@
       <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="24" t="s">
         <v>37</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="23" t="s">
         <v>38</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1909,11 +1922,11 @@
       <c r="E23"/>
     </row>
     <row r="24" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
       <c r="D24" s="18" t="s">
         <v>41</v>
       </c>
@@ -1922,11 +1935,11 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -1935,11 +1948,11 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="18" t="s">
         <v>40</v>
       </c>
@@ -1948,11 +1961,11 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="18" t="s">
         <v>42</v>
       </c>
@@ -1961,11 +1974,11 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="18">
         <v>0</v>
       </c>
@@ -1974,11 +1987,11 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="18" t="s">
         <v>43</v>
       </c>
@@ -1987,11 +2000,11 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
       <c r="D30" s="18" t="s">
         <v>44</v>
       </c>
@@ -3462,7 +3475,7 @@
       <c r="E234"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="A30:C30"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A24:C24"/>
@@ -3473,6 +3486,7 @@
     <mergeCell ref="A29:C29"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D9:E9"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
REP-64: Signatory change (#101)
* REP-64: Signatory change

* Restore InvoicesQuery.java

Co-authored-by: Inal Arsanukaev <inalarsanukaev@MacBook-Pro-Inal.local>
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/provision_of_service_act.xlsx
+++ b/src/main/resources/templates/provision_of_service_act.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tolkonepiu/Projects/reporter/src/main/resources/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/inalarsanukaev/git/reporter/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1924D5C9-7AC5-B34F-95CD-5A549C0B747F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,18 +28,18 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>Акт об оказании услуг</t>
   </si>
@@ -152,12 +153,6 @@
     <t>м.п.</t>
   </si>
   <si>
-    <t>Председатель Правления</t>
-  </si>
-  <si>
-    <t>Бурлаков К.В.</t>
-  </si>
-  <si>
     <t>${registered_name}</t>
   </si>
   <si>
@@ -204,12 +199,21 @@
   </si>
   <si>
     <t>${shop_id}</t>
+  </si>
+  <si>
+    <t>Заместитель Председателя Правления</t>
+  </si>
+  <si>
+    <t>Лебедева Л.В.</t>
+  </si>
+  <si>
+    <t>Доверенность № 13 от 21.02.2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;;&quot;-&quot;#,##0.00&quot; &quot;"/>
   </numFmts>
@@ -234,13 +238,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -248,6 +245,13 @@
     <font>
       <sz val="10"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -363,10 +367,10 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -387,7 +391,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
@@ -462,6 +466,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1571,11 +1578,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DZ234"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="160" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1595,12 +1602,12 @@
     </row>
     <row r="2" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
       <c r="D2" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E2" s="21"/>
     </row>
@@ -1637,7 +1644,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="10"/>
       <c r="E6" s="20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:130" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1779,7 +1786,7 @@
       <c r="C8" s="2"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1787,7 +1794,7 @@
       <c r="B9" s="2"/>
       <c r="C9" s="13"/>
       <c r="D9" s="30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E9" s="30"/>
     </row>
@@ -1797,7 +1804,7 @@
       <c r="C10" s="13"/>
       <c r="D10" s="19"/>
       <c r="E10" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1837,13 +1844,13 @@
         <v>8</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>10</v>
@@ -1872,7 +1879,7 @@
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>13</v>
@@ -1892,7 +1899,7 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>13</v>
@@ -1928,7 +1935,7 @@
       <c r="B24" s="25"/>
       <c r="C24" s="25"/>
       <c r="D24" s="18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>13</v>
@@ -1941,7 +1948,7 @@
       <c r="B25" s="27"/>
       <c r="C25" s="27"/>
       <c r="D25" s="18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>18</v>
@@ -1954,7 +1961,7 @@
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
       <c r="D26" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>18</v>
@@ -1967,7 +1974,7 @@
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
       <c r="D27" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>18</v>
@@ -1993,7 +2000,7 @@
       <c r="B29" s="27"/>
       <c r="C29" s="27"/>
       <c r="D29" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>13</v>
@@ -2006,7 +2013,7 @@
       <c r="B30" s="25"/>
       <c r="C30" s="25"/>
       <c r="D30" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>13</v>
@@ -2098,24 +2105,24 @@
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2131,7 +2138,7 @@
     </row>
     <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -3488,7 +3495,7 @@
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D9:E9"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter>

</xml_diff>

<commit_message>
Change sub name and position (#124)
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/provision_of_service_act.xlsx
+++ b/src/main/resources/templates/provision_of_service_act.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/inalarsanukaev/git/reporter/src/main/resources/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tolkonepiu/Projects/reporter/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1924D5C9-7AC5-B34F-95CD-5A549C0B747F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CECAEF5-5C33-E746-8521-AE4E1D68E236}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -201,13 +201,13 @@
     <t>${shop_id}</t>
   </si>
   <si>
-    <t>Заместитель Председателя Правления</t>
-  </si>
-  <si>
-    <t>Лебедева Л.В.</t>
-  </si>
-  <si>
     <t>Доверенность № 13 от 21.02.2020</t>
+  </si>
+  <si>
+    <t>Губайдулин Т.Ф.</t>
+  </si>
+  <si>
+    <t>Председатель Правления</t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1582,7 +1582,7 @@
   <dimension ref="A1:DZ234"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="160" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="D9" sqref="D9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2105,7 +2105,7 @@
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2138,7 +2138,7 @@
     </row>
     <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>

</xml_diff>

<commit_message>
BJ-999: Change signer in acts (#134)
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/provision_of_service_act.xlsx
+++ b/src/main/resources/templates/provision_of_service_act.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tolkonepiu/Projects/reporter/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F084B5F0-130A-F049-A20F-282F578A2E94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBAF213-BFA6-F345-9368-EB903AB3195D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
     <t>Акт об оказании услуг</t>
   </si>
@@ -195,19 +195,22 @@
     <t>${shop_id}</t>
   </si>
   <si>
-    <t>Председатель Правления</t>
-  </si>
-  <si>
-    <t>действующий на основании Устава</t>
-  </si>
-  <si>
-    <t>Губайдулин Т.Ф.,</t>
-  </si>
-  <si>
     <t>${representative_full_name},</t>
   </si>
   <si>
     <t>действующий на основании</t>
+  </si>
+  <si>
+    <t>Главный бухгалтер</t>
+  </si>
+  <si>
+    <t>Кахно А.В.,</t>
+  </si>
+  <si>
+    <t>действующая на основании</t>
+  </si>
+  <si>
+    <t>Доверенности N 40 от 08.09.2020</t>
   </si>
 </sst>
 </file>
@@ -1593,8 +1596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DZ234"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A24" zoomScale="160" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A30" zoomScale="160" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2117,7 +2120,7 @@
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2128,28 +2131,30 @@
     </row>
     <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="26" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="25" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="3"/>
+      <c r="A44" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>

</xml_diff>

<commit_message>
Change signer data (#145)
* Fixed function (#141)

* Fixed function

* Added new query

* Fix test

Co-authored-by: Inal Arsanukaev <inalarsanukaev@MacBook-Pro-Inal.local>

* Fix capturedAt time (#143)

Co-authored-by: Inal Arsanukaev <inalarsanukaev@MacBook-Pro-Inal.local>

* Bump damsel: uzcard added (#144)

Co-authored-by: Inal Arsanukaev <inalarsanukaev@MacBook-Pro-Inal.local>

* Bump deps

* Change signer data

Co-authored-by: Inal Arsanukaev <in.all.young@gmail.com>
Co-authored-by: Inal Arsanukaev <inalarsanukaev@MacBook-Pro-Inal.local>
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/provision_of_service_act.xlsx
+++ b/src/main/resources/templates/provision_of_service_act.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tolkonepiu/Projects/reporter/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBAF213-BFA6-F345-9368-EB903AB3195D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E95FCEC-5918-E54F-85F2-69CAE68A9083}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -210,7 +210,7 @@
     <t>действующая на основании</t>
   </si>
   <si>
-    <t>Доверенности N 40 от 08.09.2020</t>
+    <t>Доверенности № 49 от 15.09.2020</t>
   </si>
 </sst>
 </file>
@@ -1596,8 +1596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DZ234"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A30" zoomScale="160" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScale="160" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Change signer data again (#147)
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/provision_of_service_act.xlsx
+++ b/src/main/resources/templates/provision_of_service_act.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tolkonepiu/Projects/reporter/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E95FCEC-5918-E54F-85F2-69CAE68A9083}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06495F74-7FBA-6149-A7A8-B6F6D4B0E349}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -210,7 +210,7 @@
     <t>действующая на основании</t>
   </si>
   <si>
-    <t>Доверенности № 49 от 15.09.2020</t>
+    <t>Доверенности № 40 от 15.09.2020</t>
   </si>
 </sst>
 </file>
@@ -1596,8 +1596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DZ234"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScale="160" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A28" zoomScale="160" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>